<commit_message>
fix: update ToOrder function
</commit_message>
<xml_diff>
--- a/isleg-backend/uploads/orders/order.xlsx
+++ b/isleg-backend/uploads/orders/order.xlsx
@@ -20,50 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">isleg market</t>
   </si>
   <si>
-    <t xml:space="preserve">Telefon: +993 12 227475</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMO: +993 63 757422</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instagram: @isleg_market.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mail: islegmarket@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sargyt No: 220219393317</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ady: Muhammetmyrat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sargyt edilen senes: 19.02.2022 - 21:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon nomer: +99362903131 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eltip berme wagty: 13:00-17:00 (20.02.2022)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salgy: Parahat 2/4 jay 25 otag 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Töleg şekili: Nagt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bellik: Nepesow - 465228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jemi: 559.00 m.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ady</t>
   </si>
   <si>
@@ -77,12 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">Jemi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Ak reňkli) Podguznik Sleepy 3 Midi 4-9 kg (68 sany)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">180.80</t>
   </si>
   <si>
     <t xml:space="preserve">Jemi:</t>
@@ -197,7 +152,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,10 +211,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -293,9 +244,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1019520</xdr:colOff>
+      <xdr:colOff>1019160</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
+      <xdr:rowOff>82080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -309,7 +260,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="276840" y="0"/>
-          <a:ext cx="742680" cy="463320"/>
+          <a:ext cx="742320" cy="462960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -332,10 +283,10 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.85"/>
@@ -349,9 +300,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
@@ -360,9 +309,7 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
@@ -371,9 +318,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="4"/>
@@ -382,9 +327,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="4"/>
@@ -400,9 +343,7 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -429,12 +370,8 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -442,12 +379,8 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -455,12 +388,8 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -468,12 +397,8 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A12" s="12"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -491,19 +416,19 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -517,101 +442,41 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="14" t="n">
-        <v>86812062790</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>20</v>
-      </c>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="16"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="14" t="n">
-        <v>86812062790</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>20</v>
-      </c>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="14" t="n">
-        <v>86812062790</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>20</v>
-      </c>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="14" t="n">
-        <v>86812062790</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>20</v>
-      </c>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="17"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -631,8 +496,8 @@
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>